<commit_message>
Academic year added to excel sheet
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final Project\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4941BF6B-7B2A-491A-A096-85776EE1F7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997BFD40-E626-45CF-B901-55393EABE475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3ED39F4-DD7B-4779-8C56-2EB54184343A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>K S INSTITUTE OF TECHNOLOGY</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>CO5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACADEMIC YEAR	</t>
   </si>
 </sst>
 </file>
@@ -454,6 +457,57 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -503,57 +557,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,55 +876,55 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D9" sqref="D9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:19" ht="35.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="37"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="9"/>
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="12"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -967,104 +970,106 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="29"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="12"/>
     </row>
     <row r="6" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="29"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="12"/>
     </row>
     <row r="7" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="33"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="29"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="12"/>
     </row>
     <row r="9" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="A9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1081,8 +1086,8 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1120,75 +1125,75 @@
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="18"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="35"/>
     </row>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="19" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="19" t="s">
+      <c r="E13" s="37"/>
+      <c r="F13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="37"/>
+      <c r="H13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="21" t="s">
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="7" t="s">
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="8"/>
-      <c r="P13" s="7" t="s">
+      <c r="O13" s="25"/>
+      <c r="P13" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9" t="s">
+      <c r="Q13" s="25"/>
+      <c r="R13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="S13" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1231,13 +1236,13 @@
       <c r="Q14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
     </row>
     <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="6">
         <v>18</v>
       </c>
@@ -1289,33 +1294,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="L6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B12:B15"/>
@@ -1326,6 +1304,33 @@
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:O13"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="Q5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>